<commit_message>
Update use case and unit test specs
</commit_message>
<xml_diff>
--- a/31_ユースケース記述テスト仕様書(MURAシェア).xlsx
+++ b/31_ユースケース記述テスト仕様書(MURAシェア).xlsx
@@ -18,8 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -548,7 +549,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -731,6 +732,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3310,165 +3314,482 @@
       <c r="M54" s="5" t="n"/>
     </row>
     <row r="55" ht="26.45" customFormat="1" customHeight="1" s="3">
-      <c r="A55" s="28" t="n"/>
-      <c r="B55" s="21" t="n"/>
-      <c r="C55" s="33" t="n"/>
-      <c r="D55" s="27" t="n"/>
-      <c r="E55" s="27" t="n"/>
-      <c r="F55" s="33" t="n"/>
-      <c r="G55" s="6" t="n"/>
+      <c r="A55" s="28">
+        <f>MAX($A$5:A54)+1</f>
+        <v/>
+      </c>
+      <c r="B55" s="21" t="inlineStr">
+        <is>
+          <t>売り切れ商品でチャットできない</t>
+        </is>
+      </c>
+      <c r="C55" s="33" t="inlineStr">
+        <is>
+          <t>商品詳細/商品一覧のメッセージボタン</t>
+        </is>
+      </c>
+      <c r="D55" s="27" t="inlineStr">
+        <is>
+          <t>異常系</t>
+        </is>
+      </c>
+      <c r="E55" s="27" t="inlineStr">
+        <is>
+          <t>売り切れ</t>
+        </is>
+      </c>
+      <c r="F55" s="33" t="inlineStr">
+        <is>
+          <t>売り切れ商品のメッセージボタンを押下</t>
+        </is>
+      </c>
+      <c r="G55" s="6" t="inlineStr">
+        <is>
+          <t>売り切れ表示が出てチャット画面へ遷移しない</t>
+        </is>
+      </c>
       <c r="H55" s="5" t="n"/>
-      <c r="I55" s="5" t="n"/>
+      <c r="I55" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J55" s="68" t="n"/>
       <c r="K55" s="5" t="n"/>
       <c r="L55" s="5" t="n"/>
       <c r="M55" s="5" t="n"/>
     </row>
     <row r="56" ht="26.45" customFormat="1" customHeight="1" s="3">
-      <c r="A56" s="28" t="n"/>
-      <c r="B56" s="21" t="n"/>
-      <c r="C56" s="34" t="n"/>
-      <c r="D56" s="22" t="n"/>
-      <c r="E56" s="22" t="n"/>
-      <c r="F56" s="20" t="n"/>
-      <c r="G56" s="6" t="n"/>
+      <c r="A56" s="28">
+        <f>MAX($A$5:A55)+1</f>
+        <v/>
+      </c>
+      <c r="B56" s="21" t="inlineStr">
+        <is>
+          <t>レンタル中から購入する</t>
+        </is>
+      </c>
+      <c r="C56" s="34" t="inlineStr">
+        <is>
+          <t>レンタル管理（私の申請）</t>
+        </is>
+      </c>
+      <c r="D56" s="22" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E56" s="22" t="inlineStr">
+        <is>
+          <t>購入確認</t>
+        </is>
+      </c>
+      <c r="F56" s="20" t="inlineStr">
+        <is>
+          <t>レンタル中の申請で購入ボタンを押下</t>
+        </is>
+      </c>
+      <c r="G56" s="6" t="inlineStr">
+        <is>
+          <t>購入金額・レンタル期間の料金・差額の確認画面が表示される</t>
+        </is>
+      </c>
       <c r="H56" s="5" t="n"/>
-      <c r="I56" s="5" t="n"/>
+      <c r="I56" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J56" s="68" t="n"/>
       <c r="K56" s="5" t="n"/>
       <c r="L56" s="5" t="n"/>
       <c r="M56" s="5" t="n"/>
     </row>
     <row r="57" ht="15" customFormat="1" customHeight="1" s="3">
-      <c r="A57" s="28" t="n"/>
+      <c r="A57" s="28">
+        <f>MAX($A$5:A56)+1</f>
+        <v/>
+      </c>
       <c r="B57" s="21" t="n"/>
       <c r="C57" s="34" t="n"/>
-      <c r="D57" s="27" t="n"/>
-      <c r="E57" s="5" t="n"/>
-      <c r="F57" s="5" t="n"/>
-      <c r="G57" s="6" t="n"/>
+      <c r="D57" s="27" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E57" s="5" t="inlineStr">
+        <is>
+          <t>購入申請作成</t>
+        </is>
+      </c>
+      <c r="F57" s="5" t="inlineStr">
+        <is>
+          <t>確認画面で購入を確定</t>
+        </is>
+      </c>
+      <c r="G57" s="6" t="inlineStr">
+        <is>
+          <t>購入申請が作成され購入管理に表示される（支払額は差額）</t>
+        </is>
+      </c>
       <c r="H57" s="5" t="n"/>
-      <c r="I57" s="5" t="n"/>
+      <c r="I57" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J57" s="68" t="n"/>
       <c r="K57" s="5" t="n"/>
       <c r="L57" s="5" t="n"/>
       <c r="M57" s="5" t="n"/>
     </row>
     <row r="58" ht="27" customFormat="1" customHeight="1" s="3">
-      <c r="A58" s="28" t="n"/>
+      <c r="A58" s="28">
+        <f>MAX($A$5:A57)+1</f>
+        <v/>
+      </c>
       <c r="B58" s="21" t="n"/>
       <c r="C58" s="34" t="n"/>
-      <c r="D58" s="21" t="n"/>
-      <c r="E58" s="27" t="n"/>
-      <c r="F58" s="33" t="n"/>
-      <c r="G58" s="6" t="n"/>
+      <c r="D58" s="21" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E58" s="27" t="inlineStr">
+        <is>
+          <t>承認で完了</t>
+        </is>
+      </c>
+      <c r="F58" s="33" t="inlineStr">
+        <is>
+          <t>出品者がレンタル購入申請を承認</t>
+        </is>
+      </c>
+      <c r="G58" s="6" t="inlineStr">
+        <is>
+          <t>配送不要で購入完了となりレンタルが完了扱いになる</t>
+        </is>
+      </c>
       <c r="H58" s="5" t="n"/>
-      <c r="I58" s="5" t="n"/>
+      <c r="I58" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J58" s="68" t="n"/>
       <c r="K58" s="5" t="n"/>
       <c r="L58" s="5" t="n"/>
       <c r="M58" s="5" t="n"/>
     </row>
     <row r="59" ht="15" customFormat="1" customHeight="1" s="3">
-      <c r="A59" s="28" t="n"/>
+      <c r="A59" s="28">
+        <f>MAX($A$5:A58)+1</f>
+        <v/>
+      </c>
       <c r="B59" s="22" t="n"/>
       <c r="C59" s="20" t="n"/>
-      <c r="D59" s="22" t="n"/>
-      <c r="E59" s="22" t="n"/>
-      <c r="F59" s="20" t="n"/>
-      <c r="G59" s="6" t="n"/>
+      <c r="D59" s="22" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E59" s="22" t="inlineStr">
+        <is>
+          <t>完了表示</t>
+        </is>
+      </c>
+      <c r="F59" s="20" t="inlineStr">
+        <is>
+          <t>購入完了後にレンタル管理を表示</t>
+        </is>
+      </c>
+      <c r="G59" s="6" t="inlineStr">
+        <is>
+          <t>購入手続き完了と表示され、配送/購入ボタンが表示されない</t>
+        </is>
+      </c>
       <c r="H59" s="5" t="n"/>
-      <c r="I59" s="5" t="n"/>
+      <c r="I59" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J59" s="68" t="n"/>
       <c r="K59" s="5" t="n"/>
       <c r="L59" s="5" t="n"/>
       <c r="M59" s="5" t="n"/>
     </row>
     <row r="60" ht="26.45" customFormat="1" customHeight="1" s="3">
-      <c r="A60" s="28" t="n"/>
-      <c r="B60" s="27" t="n"/>
-      <c r="C60" s="6" t="n"/>
-      <c r="D60" s="5" t="n"/>
-      <c r="E60" s="5" t="n"/>
-      <c r="F60" s="5" t="n"/>
-      <c r="G60" s="6" t="n"/>
+      <c r="A60" s="28">
+        <f>MAX($A$5:A59)+1</f>
+        <v/>
+      </c>
+      <c r="B60" s="27" t="inlineStr">
+        <is>
+          <t>購入管理（受け取った注文）</t>
+        </is>
+      </c>
+      <c r="C60" s="6" t="inlineStr">
+        <is>
+          <t>受注一覧で操作</t>
+        </is>
+      </c>
+      <c r="D60" s="5" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E60" s="5" t="inlineStr">
+        <is>
+          <t>レンタル購入承認</t>
+        </is>
+      </c>
+      <c r="F60" s="5" t="inlineStr">
+        <is>
+          <t>レンタル中購入の申請を承認</t>
+        </is>
+      </c>
+      <c r="G60" s="6" t="inlineStr">
+        <is>
+          <t>承認後に配送不要で購入完了になる</t>
+        </is>
+      </c>
       <c r="H60" s="5" t="n"/>
-      <c r="I60" s="5" t="n"/>
+      <c r="I60" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J60" s="68" t="n"/>
       <c r="K60" s="5" t="n"/>
       <c r="L60" s="5" t="n"/>
       <c r="M60" s="5" t="n"/>
     </row>
     <row r="61" ht="26.45" customFormat="1" customHeight="1" s="3">
-      <c r="A61" s="28" t="n"/>
-      <c r="B61" s="21" t="n"/>
-      <c r="C61" s="33" t="n"/>
-      <c r="D61" s="27" t="n"/>
-      <c r="E61" s="27" t="n"/>
-      <c r="F61" s="33" t="n"/>
-      <c r="G61" s="6" t="n"/>
+      <c r="A61" s="28">
+        <f>MAX($A$5:A60)+1</f>
+        <v/>
+      </c>
+      <c r="B61" s="21" t="inlineStr">
+        <is>
+          <t>取引完了の非表示（受け取った申請）</t>
+        </is>
+      </c>
+      <c r="C61" s="33" t="inlineStr">
+        <is>
+          <t>レンタル管理（受け取った申請）</t>
+        </is>
+      </c>
+      <c r="D61" s="27" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E61" s="27" t="inlineStr">
+        <is>
+          <t>非表示</t>
+        </is>
+      </c>
+      <c r="F61" s="33" t="inlineStr">
+        <is>
+          <t>完了済み申請の非表示ボタンを押下</t>
+        </is>
+      </c>
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>一覧から非表示になり、取引履歴から確認できる</t>
+        </is>
+      </c>
       <c r="H61" s="5" t="n"/>
-      <c r="I61" s="5" t="n"/>
+      <c r="I61" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J61" s="68" t="n"/>
       <c r="K61" s="5" t="n"/>
       <c r="L61" s="5" t="n"/>
       <c r="M61" s="5" t="n"/>
     </row>
     <row r="62" ht="15" customFormat="1" customHeight="1" s="3">
-      <c r="A62" s="28" t="n"/>
-      <c r="B62" s="21" t="n"/>
-      <c r="C62" s="27" t="n"/>
-      <c r="D62" s="27" t="n"/>
-      <c r="E62" s="27" t="n"/>
-      <c r="F62" s="5" t="n"/>
-      <c r="G62" s="6" t="n"/>
+      <c r="A62" s="28">
+        <f>MAX($A$5:A61)+1</f>
+        <v/>
+      </c>
+      <c r="B62" s="21" t="inlineStr">
+        <is>
+          <t>取引完了の非表示（私の申請）</t>
+        </is>
+      </c>
+      <c r="C62" s="27" t="inlineStr">
+        <is>
+          <t>レンタル管理（私の申請）</t>
+        </is>
+      </c>
+      <c r="D62" s="27" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E62" s="27" t="inlineStr">
+        <is>
+          <t>非表示</t>
+        </is>
+      </c>
+      <c r="F62" s="5" t="inlineStr">
+        <is>
+          <t>完了済み申請の非表示ボタンを押下</t>
+        </is>
+      </c>
+      <c r="G62" s="6" t="inlineStr">
+        <is>
+          <t>一覧から非表示になり、取引履歴から確認できる</t>
+        </is>
+      </c>
       <c r="H62" s="5" t="n"/>
-      <c r="I62" s="5" t="n"/>
+      <c r="I62" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J62" s="68" t="n"/>
       <c r="K62" s="5" t="n"/>
       <c r="L62" s="5" t="n"/>
       <c r="M62" s="5" t="n"/>
     </row>
     <row r="63" ht="15" customFormat="1" customHeight="1" s="3">
-      <c r="A63" s="28" t="n"/>
-      <c r="B63" s="21" t="n"/>
-      <c r="C63" s="21" t="n"/>
-      <c r="D63" s="21" t="n"/>
-      <c r="E63" s="21" t="n"/>
-      <c r="F63" s="27" t="n"/>
-      <c r="G63" s="6" t="n"/>
+      <c r="A63" s="28">
+        <f>MAX($A$5:A62)+1</f>
+        <v/>
+      </c>
+      <c r="B63" s="21" t="inlineStr">
+        <is>
+          <t>取引完了の非表示（購入管理）</t>
+        </is>
+      </c>
+      <c r="C63" s="21" t="inlineStr">
+        <is>
+          <t>購入管理（私の購入/受け取った注文）</t>
+        </is>
+      </c>
+      <c r="D63" s="21" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E63" s="21" t="inlineStr">
+        <is>
+          <t>非表示</t>
+        </is>
+      </c>
+      <c r="F63" s="27" t="inlineStr">
+        <is>
+          <t>完了済みの購入に非表示ボタンを押下</t>
+        </is>
+      </c>
+      <c r="G63" s="6" t="inlineStr">
+        <is>
+          <t>一覧から非表示になり、取引履歴から確認できる</t>
+        </is>
+      </c>
       <c r="H63" s="5" t="n"/>
-      <c r="I63" s="5" t="n"/>
+      <c r="I63" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J63" s="68" t="n"/>
       <c r="K63" s="5" t="n"/>
       <c r="L63" s="5" t="n"/>
       <c r="M63" s="5" t="n"/>
     </row>
     <row r="64" ht="15" customFormat="1" customHeight="1" s="3">
-      <c r="A64" s="28" t="n"/>
-      <c r="B64" s="22" t="n"/>
-      <c r="C64" s="22" t="n"/>
-      <c r="D64" s="22" t="n"/>
-      <c r="E64" s="22" t="n"/>
-      <c r="F64" s="22" t="n"/>
-      <c r="G64" s="6" t="n"/>
+      <c r="A64" s="28">
+        <f>MAX($A$5:A63)+1</f>
+        <v/>
+      </c>
+      <c r="B64" s="22" t="inlineStr">
+        <is>
+          <t>取引完了の非表示（返品管理）</t>
+        </is>
+      </c>
+      <c r="C64" s="22" t="inlineStr">
+        <is>
+          <t>返品管理</t>
+        </is>
+      </c>
+      <c r="D64" s="22" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E64" s="22" t="inlineStr">
+        <is>
+          <t>非表示</t>
+        </is>
+      </c>
+      <c r="F64" s="22" t="inlineStr">
+        <is>
+          <t>返品完了/却下の申請に非表示ボタンを押下</t>
+        </is>
+      </c>
+      <c r="G64" s="6" t="inlineStr">
+        <is>
+          <t>一覧から非表示になり、取引履歴から確認できる</t>
+        </is>
+      </c>
       <c r="H64" s="5" t="n"/>
-      <c r="I64" s="5" t="n"/>
+      <c r="I64" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J64" s="68" t="n"/>
       <c r="K64" s="5" t="n"/>
       <c r="L64" s="5" t="n"/>
       <c r="M64" s="5" t="n"/>
     </row>
     <row r="65" ht="26.45" customFormat="1" customHeight="1" s="3">
-      <c r="A65" s="28" t="n"/>
-      <c r="B65" s="27" t="n"/>
-      <c r="C65" s="6" t="n"/>
-      <c r="D65" s="5" t="n"/>
-      <c r="E65" s="5" t="n"/>
-      <c r="F65" s="5" t="n"/>
-      <c r="G65" s="6" t="n"/>
+      <c r="A65" s="28">
+        <f>MAX($A$5:A64)+1</f>
+        <v/>
+      </c>
+      <c r="B65" s="27" t="inlineStr">
+        <is>
+          <t>会社概要を表示する</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>サイドバーの会社概要</t>
+        </is>
+      </c>
+      <c r="D65" s="5" t="inlineStr">
+        <is>
+          <t>正常系</t>
+        </is>
+      </c>
+      <c r="E65" s="5" t="inlineStr">
+        <is>
+          <t>表示</t>
+        </is>
+      </c>
+      <c r="F65" s="5" t="inlineStr">
+        <is>
+          <t>会社概要を開く</t>
+        </is>
+      </c>
+      <c r="G65" s="6" t="inlineStr">
+        <is>
+          <t>会社概要ページが表示される</t>
+        </is>
+      </c>
       <c r="H65" s="5" t="n"/>
-      <c r="I65" s="5" t="n"/>
+      <c r="I65" s="5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="J65" s="68" t="n"/>
       <c r="K65" s="5" t="n"/>
       <c r="L65" s="5" t="n"/>
@@ -4376,7 +4697,9 @@
           <t>改訂日</t>
         </is>
       </c>
-      <c r="O1" s="41" t="n"/>
+      <c r="O1" s="69" t="n">
+        <v>46044</v>
+      </c>
       <c r="P1" s="60" t="n"/>
     </row>
     <row r="2" ht="15" customHeight="1" s="56" thickBot="1">

</xml_diff>

<commit_message>
Update specs, chat list, and company info
</commit_message>
<xml_diff>
--- a/31_ユースケース記述テスト仕様書(MURAシェア).xlsx
+++ b/31_ユースケース記述テスト仕様書(MURAシェア).xlsx
@@ -1264,12 +1264,18 @@
       <c r="H5" s="5" t="n"/>
       <c r="I5" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J5" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J5" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K5" s="5" t="n"/>
-      <c r="L5" s="5" t="n"/>
+      <c r="L5" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M5" s="5" t="n"/>
     </row>
     <row r="6" ht="40.5" customFormat="1" customHeight="1" s="3">
@@ -1302,12 +1308,18 @@
       <c r="H6" s="5" t="n"/>
       <c r="I6" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J6" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J6" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K6" s="5" t="n"/>
-      <c r="L6" s="5" t="n"/>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M6" s="5" t="n"/>
       <c r="P6" s="40" t="n"/>
     </row>
@@ -1341,12 +1353,18 @@
       <c r="H7" s="5" t="n"/>
       <c r="I7" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J7" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J7" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K7" s="5" t="n"/>
-      <c r="L7" s="5" t="n"/>
+      <c r="L7" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M7" s="5" t="n"/>
       <c r="P7" s="40" t="n"/>
     </row>
@@ -1389,12 +1407,18 @@
       <c r="H8" s="5" t="n"/>
       <c r="I8" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J8" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J8" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K8" s="5" t="n"/>
-      <c r="L8" s="5" t="n"/>
+      <c r="L8" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M8" s="5" t="n"/>
     </row>
     <row r="9" ht="27" customFormat="1" customHeight="1" s="3">
@@ -1427,12 +1451,18 @@
       <c r="H9" s="5" t="n"/>
       <c r="I9" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J9" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J9" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K9" s="5" t="n"/>
-      <c r="L9" s="5" t="n"/>
+      <c r="L9" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M9" s="5" t="n"/>
     </row>
     <row r="10" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1473,12 +1503,18 @@
       <c r="H10" s="5" t="n"/>
       <c r="I10" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J10" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J10" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K10" s="5" t="n"/>
-      <c r="L10" s="5" t="n"/>
+      <c r="L10" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M10" s="5" t="n"/>
     </row>
     <row r="11" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1519,12 +1555,18 @@
       <c r="H11" s="5" t="n"/>
       <c r="I11" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J11" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J11" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K11" s="5" t="n"/>
-      <c r="L11" s="5" t="n"/>
+      <c r="L11" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M11" s="5" t="n"/>
     </row>
     <row r="12" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1557,12 +1599,18 @@
       <c r="H12" s="5" t="n"/>
       <c r="I12" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J12" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J12" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K12" s="5" t="n"/>
-      <c r="L12" s="5" t="n"/>
+      <c r="L12" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M12" s="5" t="n"/>
     </row>
     <row r="13" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1595,12 +1643,18 @@
       <c r="H13" s="5" t="n"/>
       <c r="I13" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J13" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J13" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K13" s="5" t="n"/>
-      <c r="L13" s="5" t="n"/>
+      <c r="L13" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M13" s="5" t="n"/>
     </row>
     <row r="14" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1633,12 +1687,18 @@
       <c r="H14" s="5" t="n"/>
       <c r="I14" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J14" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J14" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K14" s="5" t="n"/>
-      <c r="L14" s="5" t="n"/>
+      <c r="L14" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M14" s="5" t="n"/>
     </row>
     <row r="15" ht="39.6" customFormat="1" customHeight="1" s="3">
@@ -1679,12 +1739,18 @@
       <c r="H15" s="5" t="n"/>
       <c r="I15" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J15" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J15" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K15" s="5" t="n"/>
-      <c r="L15" s="5" t="n"/>
+      <c r="L15" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M15" s="5" t="n"/>
     </row>
     <row r="16" ht="13.15" customFormat="1" customHeight="1" s="3">
@@ -1717,12 +1783,18 @@
       <c r="H16" s="5" t="n"/>
       <c r="I16" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J16" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J16" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K16" s="5" t="n"/>
-      <c r="L16" s="5" t="n"/>
+      <c r="L16" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M16" s="5" t="n"/>
     </row>
     <row r="17" ht="39.6" customFormat="1" customHeight="1" s="3">
@@ -1763,12 +1835,18 @@
       <c r="H17" s="5" t="n"/>
       <c r="I17" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J17" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J17" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K17" s="5" t="n"/>
-      <c r="L17" s="5" t="n"/>
+      <c r="L17" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M17" s="5" t="n"/>
     </row>
     <row r="18" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1801,12 +1879,18 @@
       <c r="H18" s="5" t="n"/>
       <c r="I18" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J18" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J18" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K18" s="5" t="n"/>
-      <c r="L18" s="5" t="n"/>
+      <c r="L18" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M18" s="5" t="n"/>
     </row>
     <row r="19" ht="39.6" customFormat="1" customHeight="1" s="3">
@@ -1847,12 +1931,18 @@
       <c r="H19" s="5" t="n"/>
       <c r="I19" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J19" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J19" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K19" s="5" t="n"/>
-      <c r="L19" s="5" t="n"/>
+      <c r="L19" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M19" s="5" t="n"/>
     </row>
     <row r="20" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1885,12 +1975,18 @@
       <c r="H20" s="5" t="n"/>
       <c r="I20" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J20" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J20" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K20" s="5" t="n"/>
-      <c r="L20" s="5" t="n"/>
+      <c r="L20" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M20" s="5" t="n"/>
     </row>
     <row r="21" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -1931,12 +2027,18 @@
       <c r="H21" s="5" t="n"/>
       <c r="I21" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J21" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J21" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K21" s="5" t="n"/>
-      <c r="L21" s="5" t="n"/>
+      <c r="L21" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M21" s="5" t="n"/>
     </row>
     <row r="22" ht="54" customFormat="1" customHeight="1" s="3">
@@ -1969,12 +2071,18 @@
       <c r="H22" s="5" t="n"/>
       <c r="I22" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J22" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J22" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K22" s="5" t="n"/>
-      <c r="L22" s="5" t="n"/>
+      <c r="L22" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M22" s="5" t="n"/>
     </row>
     <row r="23" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2007,12 +2115,18 @@
       <c r="H23" s="5" t="n"/>
       <c r="I23" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J23" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J23" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K23" s="5" t="n"/>
-      <c r="L23" s="5" t="n"/>
+      <c r="L23" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M23" s="5" t="n"/>
     </row>
     <row r="24" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2053,12 +2167,18 @@
       <c r="H24" s="5" t="n"/>
       <c r="I24" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J24" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J24" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K24" s="5" t="n"/>
-      <c r="L24" s="5" t="n"/>
+      <c r="L24" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M24" s="5" t="n"/>
     </row>
     <row r="25" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2091,12 +2211,18 @@
       <c r="H25" s="5" t="n"/>
       <c r="I25" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J25" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J25" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K25" s="5" t="n"/>
-      <c r="L25" s="5" t="n"/>
+      <c r="L25" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M25" s="5" t="n"/>
     </row>
     <row r="26" ht="27" customFormat="1" customHeight="1" s="3">
@@ -2137,12 +2263,18 @@
       <c r="H26" s="5" t="n"/>
       <c r="I26" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J26" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J26" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K26" s="5" t="n"/>
-      <c r="L26" s="5" t="n"/>
+      <c r="L26" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M26" s="5" t="n"/>
     </row>
     <row r="27" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2175,12 +2307,18 @@
       <c r="H27" s="5" t="n"/>
       <c r="I27" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J27" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J27" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K27" s="5" t="n"/>
-      <c r="L27" s="5" t="n"/>
+      <c r="L27" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M27" s="5" t="n"/>
     </row>
     <row r="28" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2221,12 +2359,18 @@
       <c r="H28" s="5" t="n"/>
       <c r="I28" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J28" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J28" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K28" s="5" t="n"/>
-      <c r="L28" s="5" t="n"/>
+      <c r="L28" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M28" s="5" t="n"/>
     </row>
     <row r="29" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2259,12 +2403,18 @@
       <c r="H29" s="5" t="n"/>
       <c r="I29" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J29" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J29" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K29" s="5" t="n"/>
-      <c r="L29" s="5" t="n"/>
+      <c r="L29" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M29" s="5" t="n"/>
     </row>
     <row r="30" ht="27" customFormat="1" customHeight="1" s="3">
@@ -2297,12 +2447,18 @@
       <c r="H30" s="5" t="n"/>
       <c r="I30" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J30" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J30" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K30" s="5" t="n"/>
-      <c r="L30" s="5" t="n"/>
+      <c r="L30" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M30" s="5" t="n"/>
     </row>
     <row r="31" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2343,12 +2499,18 @@
       <c r="H31" s="5" t="n"/>
       <c r="I31" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J31" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J31" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K31" s="5" t="n"/>
-      <c r="L31" s="5" t="n"/>
+      <c r="L31" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M31" s="5" t="n"/>
     </row>
     <row r="32" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2381,12 +2543,18 @@
       <c r="H32" s="5" t="n"/>
       <c r="I32" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J32" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J32" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K32" s="5" t="n"/>
-      <c r="L32" s="5" t="n"/>
+      <c r="L32" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M32" s="5" t="n"/>
     </row>
     <row r="33" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2419,12 +2587,18 @@
       <c r="H33" s="5" t="n"/>
       <c r="I33" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J33" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J33" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K33" s="5" t="n"/>
-      <c r="L33" s="5" t="n"/>
+      <c r="L33" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M33" s="5" t="n"/>
     </row>
     <row r="34" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2465,12 +2639,18 @@
       <c r="H34" s="5" t="n"/>
       <c r="I34" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J34" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J34" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K34" s="5" t="n"/>
-      <c r="L34" s="5" t="n"/>
+      <c r="L34" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M34" s="5" t="n"/>
     </row>
     <row r="35" ht="27" customFormat="1" customHeight="1" s="3">
@@ -2503,12 +2683,18 @@
       <c r="H35" s="5" t="n"/>
       <c r="I35" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J35" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J35" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K35" s="5" t="n"/>
-      <c r="L35" s="5" t="n"/>
+      <c r="L35" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M35" s="5" t="n"/>
     </row>
     <row r="36" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2549,12 +2735,18 @@
       <c r="H36" s="5" t="n"/>
       <c r="I36" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J36" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J36" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K36" s="5" t="n"/>
-      <c r="L36" s="5" t="n"/>
+      <c r="L36" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M36" s="5" t="n"/>
     </row>
     <row r="37" ht="39.6" customFormat="1" customHeight="1" s="3">
@@ -2587,12 +2779,18 @@
       <c r="H37" s="5" t="n"/>
       <c r="I37" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J37" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J37" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K37" s="5" t="n"/>
-      <c r="L37" s="5" t="n"/>
+      <c r="L37" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M37" s="5" t="n"/>
     </row>
     <row r="38" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2633,12 +2831,18 @@
       <c r="H38" s="5" t="n"/>
       <c r="I38" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J38" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J38" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K38" s="5" t="n"/>
-      <c r="L38" s="5" t="n"/>
+      <c r="L38" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M38" s="5" t="n"/>
     </row>
     <row r="39" ht="15" customFormat="1" customHeight="1" s="3">
@@ -2671,12 +2875,18 @@
       <c r="H39" s="5" t="n"/>
       <c r="I39" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J39" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J39" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K39" s="5" t="n"/>
-      <c r="L39" s="5" t="n"/>
+      <c r="L39" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M39" s="5" t="n"/>
     </row>
     <row r="40" ht="13.15" customFormat="1" customHeight="1" s="3">
@@ -2717,12 +2927,18 @@
       <c r="H40" s="5" t="n"/>
       <c r="I40" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J40" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J40" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K40" s="5" t="n"/>
-      <c r="L40" s="5" t="n"/>
+      <c r="L40" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M40" s="5" t="n"/>
     </row>
     <row r="41" ht="27" customFormat="1" customHeight="1" s="3">
@@ -2755,12 +2971,18 @@
       <c r="H41" s="5" t="n"/>
       <c r="I41" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J41" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J41" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K41" s="5" t="n"/>
-      <c r="L41" s="5" t="n"/>
+      <c r="L41" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M41" s="5" t="n"/>
     </row>
     <row r="42" ht="15" customFormat="1" customHeight="1" s="3">
@@ -2793,12 +3015,18 @@
       <c r="H42" s="5" t="n"/>
       <c r="I42" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J42" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J42" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K42" s="5" t="n"/>
-      <c r="L42" s="5" t="n"/>
+      <c r="L42" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M42" s="5" t="n"/>
     </row>
     <row r="43" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2831,12 +3059,18 @@
       <c r="H43" s="5" t="n"/>
       <c r="I43" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J43" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J43" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K43" s="5" t="n"/>
-      <c r="L43" s="5" t="n"/>
+      <c r="L43" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M43" s="5" t="n"/>
     </row>
     <row r="44" ht="15" customFormat="1" customHeight="1" s="3">
@@ -2877,12 +3111,18 @@
       <c r="H44" s="5" t="n"/>
       <c r="I44" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J44" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J44" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K44" s="5" t="n"/>
-      <c r="L44" s="5" t="n"/>
+      <c r="L44" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M44" s="5" t="n"/>
     </row>
     <row r="45" ht="40.5" customFormat="1" customHeight="1" s="3">
@@ -2915,12 +3155,18 @@
       <c r="H45" s="5" t="n"/>
       <c r="I45" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J45" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J45" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K45" s="5" t="n"/>
-      <c r="L45" s="5" t="n"/>
+      <c r="L45" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M45" s="5" t="n"/>
     </row>
     <row r="46" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -2953,12 +3199,18 @@
       <c r="H46" s="5" t="n"/>
       <c r="I46" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J46" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J46" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K46" s="5" t="n"/>
-      <c r="L46" s="5" t="n"/>
+      <c r="L46" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M46" s="5" t="n"/>
     </row>
     <row r="47" ht="15" customFormat="1" customHeight="1" s="3">
@@ -2991,12 +3243,18 @@
       <c r="H47" s="5" t="n"/>
       <c r="I47" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J47" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J47" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K47" s="5" t="n"/>
-      <c r="L47" s="5" t="n"/>
+      <c r="L47" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M47" s="5" t="n"/>
     </row>
     <row r="48" ht="27" customFormat="1" customHeight="1" s="3">
@@ -3037,12 +3295,18 @@
       <c r="H48" s="5" t="n"/>
       <c r="I48" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J48" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J48" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K48" s="5" t="n"/>
-      <c r="L48" s="5" t="n"/>
+      <c r="L48" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M48" s="5" t="n"/>
     </row>
     <row r="49" ht="15" customFormat="1" customHeight="1" s="3">
@@ -3083,12 +3347,18 @@
       <c r="H49" s="5" t="n"/>
       <c r="I49" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J49" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J49" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K49" s="5" t="n"/>
-      <c r="L49" s="5" t="n"/>
+      <c r="L49" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M49" s="5" t="n"/>
     </row>
     <row r="50" ht="40.5" customFormat="1" customHeight="1" s="3">
@@ -3129,12 +3399,18 @@
       <c r="H50" s="5" t="n"/>
       <c r="I50" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J50" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J50" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K50" s="5" t="n"/>
-      <c r="L50" s="5" t="n"/>
+      <c r="L50" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M50" s="5" t="n"/>
     </row>
     <row r="51" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3175,12 +3451,18 @@
       <c r="H51" s="5" t="n"/>
       <c r="I51" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J51" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J51" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K51" s="5" t="n"/>
-      <c r="L51" s="5" t="n"/>
+      <c r="L51" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M51" s="5" t="n"/>
     </row>
     <row r="52" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3213,12 +3495,18 @@
       <c r="H52" s="5" t="n"/>
       <c r="I52" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J52" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J52" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K52" s="5" t="n"/>
-      <c r="L52" s="5" t="n"/>
+      <c r="L52" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M52" s="5" t="n"/>
     </row>
     <row r="53" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3259,12 +3547,18 @@
       <c r="H53" s="5" t="n"/>
       <c r="I53" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J53" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J53" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K53" s="5" t="n"/>
-      <c r="L53" s="5" t="n"/>
+      <c r="L53" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M53" s="5" t="n"/>
     </row>
     <row r="54" ht="15" customFormat="1" customHeight="1" s="3">
@@ -3305,12 +3599,18 @@
       <c r="H54" s="5" t="n"/>
       <c r="I54" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J54" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J54" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K54" s="5" t="n"/>
-      <c r="L54" s="5" t="n"/>
+      <c r="L54" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M54" s="5" t="n"/>
     </row>
     <row r="55" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3351,12 +3651,18 @@
       <c r="H55" s="5" t="n"/>
       <c r="I55" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J55" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J55" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K55" s="5" t="n"/>
-      <c r="L55" s="5" t="n"/>
+      <c r="L55" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M55" s="5" t="n"/>
     </row>
     <row r="56" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3397,12 +3703,18 @@
       <c r="H56" s="5" t="n"/>
       <c r="I56" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J56" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J56" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K56" s="5" t="n"/>
-      <c r="L56" s="5" t="n"/>
+      <c r="L56" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M56" s="5" t="n"/>
     </row>
     <row r="57" ht="15" customFormat="1" customHeight="1" s="3">
@@ -3435,12 +3747,18 @@
       <c r="H57" s="5" t="n"/>
       <c r="I57" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J57" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J57" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K57" s="5" t="n"/>
-      <c r="L57" s="5" t="n"/>
+      <c r="L57" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M57" s="5" t="n"/>
     </row>
     <row r="58" ht="27" customFormat="1" customHeight="1" s="3">
@@ -3473,12 +3791,18 @@
       <c r="H58" s="5" t="n"/>
       <c r="I58" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J58" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J58" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K58" s="5" t="n"/>
-      <c r="L58" s="5" t="n"/>
+      <c r="L58" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M58" s="5" t="n"/>
     </row>
     <row r="59" ht="15" customFormat="1" customHeight="1" s="3">
@@ -3511,12 +3835,18 @@
       <c r="H59" s="5" t="n"/>
       <c r="I59" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J59" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J59" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K59" s="5" t="n"/>
-      <c r="L59" s="5" t="n"/>
+      <c r="L59" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M59" s="5" t="n"/>
     </row>
     <row r="60" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3557,12 +3887,18 @@
       <c r="H60" s="5" t="n"/>
       <c r="I60" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J60" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J60" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K60" s="5" t="n"/>
-      <c r="L60" s="5" t="n"/>
+      <c r="L60" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M60" s="5" t="n"/>
     </row>
     <row r="61" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3603,12 +3939,18 @@
       <c r="H61" s="5" t="n"/>
       <c r="I61" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J61" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J61" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K61" s="5" t="n"/>
-      <c r="L61" s="5" t="n"/>
+      <c r="L61" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M61" s="5" t="n"/>
     </row>
     <row r="62" ht="15" customFormat="1" customHeight="1" s="3">
@@ -3649,12 +3991,18 @@
       <c r="H62" s="5" t="n"/>
       <c r="I62" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J62" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J62" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K62" s="5" t="n"/>
-      <c r="L62" s="5" t="n"/>
+      <c r="L62" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M62" s="5" t="n"/>
     </row>
     <row r="63" ht="15" customFormat="1" customHeight="1" s="3">
@@ -3695,12 +4043,18 @@
       <c r="H63" s="5" t="n"/>
       <c r="I63" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J63" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J63" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K63" s="5" t="n"/>
-      <c r="L63" s="5" t="n"/>
+      <c r="L63" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M63" s="5" t="n"/>
     </row>
     <row r="64" ht="15" customFormat="1" customHeight="1" s="3">
@@ -3741,12 +4095,18 @@
       <c r="H64" s="5" t="n"/>
       <c r="I64" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J64" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J64" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K64" s="5" t="n"/>
-      <c r="L64" s="5" t="n"/>
+      <c r="L64" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M64" s="5" t="n"/>
     </row>
     <row r="65" ht="26.45" customFormat="1" customHeight="1" s="3">
@@ -3787,12 +4147,18 @@
       <c r="H65" s="5" t="n"/>
       <c r="I65" s="5" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J65" s="68" t="n"/>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="J65" s="68" t="n">
+        <v>46045</v>
+      </c>
       <c r="K65" s="5" t="n"/>
-      <c r="L65" s="5" t="n"/>
+      <c r="L65" s="5" t="inlineStr">
+        <is>
+          <t>清山</t>
+        </is>
+      </c>
       <c r="M65" s="5" t="n"/>
     </row>
     <row r="66" ht="39.6" customFormat="1" customHeight="1" s="3">

</xml_diff>

<commit_message>
feat: redesign UI and update guides
</commit_message>
<xml_diff>
--- a/31_ユースケース記述テスト仕様書(MURAシェア).xlsx
+++ b/31_ユースケース記述テスト仕様書(MURAシェア).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web_app\mura_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B542C8-0A8A-43A7-86A6-7399F0DBA470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5717463A-EABA-4F53-997B-01659ED93931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="279">
   <si>
     <t>ユースケース記述テスト仕様書</t>
   </si>
@@ -45,7 +45,7 @@
     <t>システム名称</t>
   </si>
   <si>
-    <t>MURAシェア</t>
+    <t>このシステム</t>
   </si>
   <si>
     <t>改訂日</t>
@@ -308,18 +308,12 @@
     <t>投稿成功</t>
   </si>
   <si>
-    <t>必須項目と画像を入力し送信</t>
-  </si>
-  <si>
     <t>商品が作成され商品一覧に遷移</t>
   </si>
   <si>
     <t>住所未登録</t>
   </si>
   <si>
-    <t>プロフィール住所未登録で投稿画面へアクセス</t>
-  </si>
-  <si>
     <t>プロフィールへ遷移し住所登録の警告</t>
   </si>
   <si>
@@ -774,9 +768,6 @@
   </si>
   <si>
     <t>完了済みの購入に非表示ボタンを押下</t>
-  </si>
-  <si>
-    <t>取引完了の非表示（返品管理）</t>
   </si>
   <si>
     <t>返品完了/却下の申請に非表示ボタンを押下</t>
@@ -823,6 +814,174 @@
   </si>
   <si>
     <t>再試要否</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>取引完了の非表示（返品管理）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>取引履歴を確認する</t>
+    <rPh sb="0" eb="4">
+      <t>トリヒキリレキ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レビューの投稿</t>
+    <rPh sb="5" eb="7">
+      <t>トウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正常系</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>必須項目と画像を入力し送信</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロフィール住所未登録で投稿画面へアクセス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正常系</t>
+    <rPh sb="0" eb="3">
+      <t>セイジョウケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">プルダウン式で★1～5の評価を選択
+</t>
+    <rPh sb="5" eb="6">
+      <t>シキ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ヒョウカ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>センタク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">評価
+</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">商品詳細に★の5段階評価が表示される
+</t>
+    <rPh sb="0" eb="2">
+      <t>ショウヒン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t>ダンカイヒョウカ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>商品一覧ページ表示する</t>
+  </si>
+  <si>
+    <t>操作</t>
+  </si>
+  <si>
+    <t>ページネーション(1画面15商品)</t>
+  </si>
+  <si>
+    <t>1.2.3…前へ次へを押下</t>
+  </si>
+  <si>
+    <t>次前ページの商品が表示される</t>
+  </si>
+  <si>
+    <t>投稿条件・権限</t>
+    <rPh sb="0" eb="2">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジョウケン</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ケンゲン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表示・集計の反映</t>
+    <rPh sb="3" eb="5">
+      <t>シュウケイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ハンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>商品詳細でレビュー一覧・平均評価が反映</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>更新</t>
+    <rPh sb="0" eb="2">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿・更新フロー</t>
+    <rPh sb="0" eb="2">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>初回投稿成功・既存レビューがある場合は更新扱い</t>
+    <rPh sb="0" eb="6">
+      <t>ショカイトウコウセイコウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>キゾン</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>コウシンアツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿成功</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿完了後、購入者／借り手のみ投稿可</t>
+    <rPh sb="0" eb="4">
+      <t>トウコウカンリョウ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ゴ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1444,6 +1603,9 @@
     <xf numFmtId="176" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1478,9 +1640,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1768,15 +1927,14 @@
   </sheetPr>
   <dimension ref="A1:P121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="105" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="D55" zoomScale="148" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
+    <col min="2" max="3" width="30.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="21.125" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="45.875" style="1" customWidth="1"/>
@@ -1790,48 +1948,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="60" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="51"/>
+      <c r="G1" s="52"/>
       <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="62">
+      <c r="I1" s="63">
         <v>46044</v>
       </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="65"/>
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="54"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="60"/>
     </row>
     <row r="3" spans="1:16" ht="12.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1860,7 +2018,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>14</v>
@@ -2160,7 +2318,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M12" s="5"/>
     </row>
@@ -2401,7 +2559,7 @@
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J19" s="48">
         <v>46049</v>
@@ -2410,7 +2568,7 @@
         <v>82</v>
       </c>
       <c r="L19" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M19" s="5"/>
     </row>
@@ -2435,7 +2593,7 @@
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J20" s="48">
         <v>46049</v>
@@ -2444,7 +2602,7 @@
         <v>82</v>
       </c>
       <c r="L20" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M20" s="5"/>
     </row>
@@ -2466,14 +2624,14 @@
         <v>88</v>
       </c>
       <c r="F21" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J21" s="48">
         <v>46045</v>
@@ -2497,17 +2655,17 @@
         <v>26</v>
       </c>
       <c r="E22" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J22" s="48">
         <v>46045</v>
@@ -2531,17 +2689,17 @@
         <v>26</v>
       </c>
       <c r="E23" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J23" s="48">
         <v>46045</v>
@@ -2560,26 +2718,26 @@
         <v>20</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D24" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J24" s="48">
         <v>46049</v>
@@ -2588,7 +2746,7 @@
         <v>25</v>
       </c>
       <c r="L24" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M24" s="5"/>
     </row>
@@ -2603,17 +2761,17 @@
         <v>26</v>
       </c>
       <c r="E25" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J25" s="48">
         <v>46045</v>
@@ -2632,26 +2790,26 @@
         <v>22</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D26" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J26" s="48">
         <v>46045</v>
@@ -2675,17 +2833,17 @@
         <v>26</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J27" s="48">
         <v>46045</v>
@@ -2704,26 +2862,26 @@
         <v>24</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28" s="35" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J28" s="48">
         <v>46045</v>
@@ -2747,17 +2905,17 @@
         <v>26</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J29" s="48">
         <v>46045</v>
@@ -2781,17 +2939,17 @@
         <v>26</v>
       </c>
       <c r="E30" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J30" s="48">
         <v>46045</v>
@@ -2810,26 +2968,26 @@
         <v>27</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D31" s="37" t="s">
         <v>20</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J31" s="48">
         <v>46045</v>
@@ -2853,17 +3011,17 @@
         <v>26</v>
       </c>
       <c r="E32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J32" s="48">
         <v>46045</v>
@@ -2887,17 +3045,17 @@
         <v>26</v>
       </c>
       <c r="E33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J33" s="48">
         <v>46045</v>
@@ -2916,26 +3074,26 @@
         <v>30</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D34" s="37" t="s">
         <v>20</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>137</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J34" s="48">
         <v>46045</v>
@@ -2959,17 +3117,17 @@
         <v>20</v>
       </c>
       <c r="E35" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="F35" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J35" s="48">
         <v>46045</v>
@@ -2988,26 +3146,26 @@
         <v>32</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>20</v>
       </c>
       <c r="E36" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J36" s="48">
         <v>46045</v>
@@ -3031,17 +3189,17 @@
         <v>20</v>
       </c>
       <c r="E37" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J37" s="48">
         <v>46045</v>
@@ -3060,26 +3218,26 @@
         <v>34</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D38" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="F38" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J38" s="48">
         <v>46045</v>
@@ -3103,17 +3261,17 @@
         <v>20</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J39" s="48">
         <v>46045</v>
@@ -3132,26 +3290,26 @@
         <v>36</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E40" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J40" s="48">
         <v>46045</v>
@@ -3175,17 +3333,17 @@
         <v>20</v>
       </c>
       <c r="E41" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="F41" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J41" s="48">
         <v>46045</v>
@@ -3209,17 +3367,17 @@
         <v>20</v>
       </c>
       <c r="E42" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J42" s="48">
         <v>46045</v>
@@ -3243,17 +3401,17 @@
         <v>20</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J43" s="48">
         <v>46045</v>
@@ -3272,26 +3430,26 @@
         <v>40</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E44" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J44" s="48">
         <v>46045</v>
@@ -3315,17 +3473,17 @@
         <v>20</v>
       </c>
       <c r="E45" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="G45" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="F45" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J45" s="48">
         <v>46049</v>
@@ -3334,7 +3492,7 @@
         <v>5</v>
       </c>
       <c r="L45" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M45" s="5"/>
     </row>
@@ -3349,17 +3507,17 @@
         <v>20</v>
       </c>
       <c r="E46" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="G46" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J46" s="48">
         <v>46045</v>
@@ -3383,17 +3541,17 @@
         <v>20</v>
       </c>
       <c r="E47" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G47" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J47" s="48">
         <v>46049</v>
@@ -3402,7 +3560,7 @@
         <v>5</v>
       </c>
       <c r="L47" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M47" s="5"/>
     </row>
@@ -3412,26 +3570,26 @@
         <v>44</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C48" s="33" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E48" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="F48" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J48" s="48">
         <v>46045</v>
@@ -3450,26 +3608,26 @@
         <v>45</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D49" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E49" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="F49" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J49" s="48">
         <v>46045</v>
@@ -3488,26 +3646,26 @@
         <v>46</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D50" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E50" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="F50" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J50" s="48">
         <v>46045</v>
@@ -3526,32 +3684,32 @@
         <v>47</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D51" s="22" t="s">
         <v>20</v>
       </c>
       <c r="E51" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J51" s="48">
         <v>46045</v>
       </c>
       <c r="K51" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L51" s="47" t="s">
         <v>25</v>
@@ -3569,23 +3727,23 @@
         <v>26</v>
       </c>
       <c r="E52" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G52" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J52" s="48">
         <v>46045</v>
       </c>
       <c r="K52" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L52" s="47" t="s">
         <v>25</v>
@@ -3598,26 +3756,26 @@
         <v>49</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D53" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E53" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="F53" s="32" t="s">
-        <v>207</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J53" s="48">
         <v>46049</v>
@@ -3626,7 +3784,7 @@
         <v>5</v>
       </c>
       <c r="L53" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M53" s="5"/>
     </row>
@@ -3636,26 +3794,26 @@
         <v>50</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D54" s="22" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J54" s="48">
         <v>46049</v>
@@ -3664,7 +3822,7 @@
         <v>25</v>
       </c>
       <c r="L54" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M54" s="5"/>
     </row>
@@ -3674,35 +3832,35 @@
         <v>51</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D55" s="27" t="s">
         <v>26</v>
       </c>
       <c r="E55" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="G55" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="F55" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J55" s="48">
         <v>46049</v>
       </c>
       <c r="K55" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L55" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M55" s="5"/>
     </row>
@@ -3712,26 +3870,26 @@
         <v>52</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>20</v>
       </c>
       <c r="E56" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G56" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="F56" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J56" s="48">
         <v>46049</v>
@@ -3740,7 +3898,7 @@
         <v>25</v>
       </c>
       <c r="L56" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M56" s="5"/>
     </row>
@@ -3755,17 +3913,17 @@
         <v>20</v>
       </c>
       <c r="E57" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G57" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J57" s="48">
         <v>46049</v>
@@ -3773,8 +3931,8 @@
       <c r="K57" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="L57" s="68" t="s">
-        <v>256</v>
+      <c r="L57" s="49" t="s">
+        <v>253</v>
       </c>
       <c r="M57" s="5"/>
     </row>
@@ -3789,17 +3947,17 @@
         <v>20</v>
       </c>
       <c r="E58" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="G58" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F58" s="32" t="s">
-        <v>228</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="H58" s="5"/>
-      <c r="I58" s="68" t="s">
-        <v>255</v>
+      <c r="I58" s="49" t="s">
+        <v>252</v>
       </c>
       <c r="J58" s="48">
         <v>46049</v>
@@ -3808,7 +3966,7 @@
         <v>25</v>
       </c>
       <c r="L58" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M58" s="5"/>
     </row>
@@ -3823,17 +3981,17 @@
         <v>20</v>
       </c>
       <c r="E59" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G59" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J59" s="48">
         <v>46049</v>
@@ -3842,7 +4000,7 @@
         <v>25</v>
       </c>
       <c r="L59" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M59" s="5"/>
     </row>
@@ -3852,26 +4010,26 @@
         <v>56</v>
       </c>
       <c r="B60" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E60" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="G60" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="F60" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>235</v>
-      </c>
       <c r="H60" s="5"/>
-      <c r="I60" s="68" t="s">
-        <v>255</v>
+      <c r="I60" s="49" t="s">
+        <v>252</v>
       </c>
       <c r="J60" s="48">
         <v>46049</v>
@@ -3880,7 +4038,7 @@
         <v>25</v>
       </c>
       <c r="L60" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M60" s="5"/>
     </row>
@@ -3890,26 +4048,26 @@
         <v>57</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D61" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E61" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="F61" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="F61" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J61" s="48">
         <v>46045</v>
@@ -3918,7 +4076,7 @@
         <v>25</v>
       </c>
       <c r="L61" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M61" s="5"/>
     </row>
@@ -3928,26 +4086,26 @@
         <v>58</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D62" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E62" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J62" s="48">
         <v>46045</v>
@@ -3956,7 +4114,7 @@
         <v>25</v>
       </c>
       <c r="L62" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M62" s="5"/>
     </row>
@@ -3966,26 +4124,26 @@
         <v>59</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D63" s="21" t="s">
         <v>20</v>
       </c>
       <c r="E63" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F63" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="G63" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="F63" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J63" s="48">
         <v>46045</v>
@@ -3994,7 +4152,7 @@
         <v>25</v>
       </c>
       <c r="L63" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M63" s="5"/>
     </row>
@@ -4004,26 +4162,26 @@
         <v>60</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>20</v>
       </c>
       <c r="E64" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="F64" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="G64" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="F64" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="47" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J64" s="48">
         <v>46045</v>
@@ -4032,7 +4190,7 @@
         <v>25</v>
       </c>
       <c r="L64" s="47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M64" s="5"/>
     </row>
@@ -4042,76 +4200,120 @@
         <v>61</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="47" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J65" s="48">
         <v>46045</v>
       </c>
       <c r="K65" s="47" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L65" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="M65" s="5"/>
+    </row>
+    <row r="66" spans="1:13" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="28"/>
+      <c r="B66" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="M65" s="5"/>
-    </row>
-    <row r="66" spans="1:13" s="3" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="28"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="32"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="6"/>
+      <c r="C66" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>265</v>
+      </c>
       <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="7"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
+      <c r="I66" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="J66" s="48">
+        <v>46057</v>
+      </c>
+      <c r="K66" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="L66" s="47" t="s">
+        <v>254</v>
+      </c>
       <c r="M66" s="5"/>
     </row>
-    <row r="67" spans="1:13" s="3" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:13" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="28"/>
       <c r="B67" s="21"/>
       <c r="C67" s="33"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="6"/>
+      <c r="D67" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>273</v>
+      </c>
       <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
+      <c r="I67" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="J67" s="48">
+        <v>46057</v>
+      </c>
+      <c r="K67" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="L67" s="47" t="s">
+        <v>254</v>
+      </c>
       <c r="M67" s="5"/>
     </row>
-    <row r="68" spans="1:13" s="3" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:13" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="28"/>
       <c r="B68" s="21"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>276</v>
+      </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="7"/>
@@ -4119,14 +4321,22 @@
       <c r="L68" s="5"/>
       <c r="M68" s="5"/>
     </row>
-    <row r="69" spans="1:13" s="3" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:13" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="28"/>
       <c r="B69" s="21"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="6"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E69" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>278</v>
+      </c>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="7"/>
@@ -4136,12 +4346,24 @@
     </row>
     <row r="70" spans="1:13" s="3" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="28"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="6"/>
+      <c r="B70" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>270</v>
+      </c>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="7"/>
@@ -4946,52 +5168,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="49" t="s">
-        <v>252</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="60" t="s">
+      <c r="A1" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="67" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="52"/>
       <c r="N1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="66">
+      <c r="O1" s="67">
         <v>46044</v>
       </c>
-      <c r="P1" s="64"/>
+      <c r="P1" s="65"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="55"/>
       <c r="N2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="65"/>
-      <c r="P2" s="59"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="60"/>
     </row>
     <row r="3" spans="1:16" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:16" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -5015,7 +5237,7 @@
     <row r="5" spans="1:16" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P5" s="14"/>
     </row>

</xml_diff>